<commit_message>
Loads a custom report from a spreadsheet
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankreport.xlsx
+++ b/fieldManagerClient/WebContent/blankreport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Current data and time</t>
   </si>
   <si>
-    <t>is empty</t>
-  </si>
-  <si>
     <t>True if the column does not have a value</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>The value to be used if the condition is met, or the choice value for a choice row type</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>and</t>
   </si>
 </sst>
 </file>
@@ -741,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -818,10 +821,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -865,7 +868,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
@@ -877,7 +880,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -930,13 +933,13 @@
     <row r="20" spans="1:5" ht="30">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -944,7 +947,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="5"/>
@@ -959,13 +962,13 @@
     <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="5"/>
     </row>
@@ -973,7 +976,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="5"/>
@@ -1050,7 +1053,7 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1064,11 +1067,11 @@
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1076,7 +1079,7 @@
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="5"/>
@@ -1085,7 +1088,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="5"/>
@@ -1094,7 +1097,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="5"/>
@@ -1103,7 +1106,7 @@
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="5"/>
@@ -1199,10 +1202,10 @@
       <c r="A48" s="1"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -1210,17 +1213,19 @@
       <c r="A49" s="1"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+      <c r="C50" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
     </row>
@@ -1322,10 +1327,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>2</v>
@@ -1337,7 +1342,7 @@
         <v>29</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1"/>
       <c r="L1"/>
@@ -2132,10 +2137,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>2</v>
@@ -2147,7 +2152,7 @@
         <v>29</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1"/>
       <c r="L1"/>
@@ -2217,7 +2222,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4"/>
       <c r="L4"/>
@@ -2244,7 +2249,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>10</v>
@@ -2271,7 +2276,7 @@
         <v>40</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6"/>
       <c r="L6"/>
@@ -2295,7 +2300,7 @@
         <v>39</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
@@ -2319,7 +2324,7 @@
         <v>42</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K8"/>
       <c r="L8"/>
@@ -2337,13 +2342,13 @@
         <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9"/>
       <c r="L9"/>
@@ -2361,13 +2366,13 @@
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -2388,10 +2393,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
@@ -2409,13 +2414,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="K12"/>
       <c r="L12"/>
@@ -2430,10 +2435,10 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
@@ -2448,10 +2453,10 @@
     </row>
     <row r="14" spans="1:20" ht="30">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K14"/>
       <c r="L14"/>
@@ -2472,7 +2477,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Selecting managed survey from a list
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankreport.xlsx
+++ b/fieldManagerClient/WebContent/blankreport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="83">
   <si>
     <t>name</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>and</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Settings Work Sheet</t>
+  </si>
+  <si>
+    <t>Set the report type. Use "oversight' for an oversight report, otherwise use your own convention to cateogorise the reports</t>
   </si>
 </sst>
 </file>
@@ -359,8 +368,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -383,6 +393,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -742,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -754,515 +767,556 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+      <c r="D26" s="3"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="D29" s="3"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2" t="s">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2" t="s">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
+      <c r="D42" s="3"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1"/>
-      <c r="B40" s="6" t="s">
+      <c r="D43" s="3"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2"/>
+      <c r="B45" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6" t="s">
+      <c r="D45" s="7"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
+      <c r="D46" s="7"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
+      <c r="D47" s="7"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6" t="s">
+      <c r="D48" s="7"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6" t="s">
+      <c r="D49" s="7"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D50" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6" t="s">
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D51" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6" t="s">
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D52" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6" t="s">
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D53" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6" t="s">
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D54" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6" t="s">
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1278,10 +1332,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1301,47 +1361,47 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="32.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="32.83203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="17.6640625" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="14" width="75.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="32.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20" style="2" customWidth="1"/>
+    <col min="5" max="6" width="9.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="32.83203125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="17.6640625" style="2" customWidth="1"/>
+    <col min="11" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="75.6640625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>75</v>
       </c>
       <c r="K1"/>
@@ -1366,11 +1426,11 @@
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3"/>
@@ -1388,11 +1448,11 @@
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4"/>
@@ -1410,11 +1470,11 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5"/>
@@ -1432,11 +1492,11 @@
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6"/>
@@ -1454,11 +1514,11 @@
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7"/>
@@ -1476,11 +1536,11 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8"/>
@@ -1498,11 +1558,11 @@
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9"/>
@@ -1520,11 +1580,11 @@
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10"/>
@@ -1542,11 +1602,11 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11"/>
@@ -1564,11 +1624,11 @@
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12"/>
@@ -1586,11 +1646,11 @@
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13"/>
@@ -1608,11 +1668,11 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14"/>
@@ -1630,11 +1690,11 @@
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15"/>
@@ -1652,11 +1712,11 @@
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16"/>
@@ -1674,11 +1734,11 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17"/>
@@ -1696,11 +1756,11 @@
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
     </row>
     <row r="18" spans="1:20">
       <c r="K18"/>
@@ -1708,11 +1768,11 @@
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
     </row>
     <row r="19" spans="1:20">
       <c r="K19"/>
@@ -1720,11 +1780,11 @@
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
     </row>
     <row r="20" spans="1:20">
       <c r="K20"/>
@@ -1732,11 +1792,11 @@
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
     </row>
     <row r="21" spans="1:20">
       <c r="K21"/>
@@ -1744,11 +1804,11 @@
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
     </row>
     <row r="22" spans="1:20">
       <c r="K22"/>
@@ -1756,11 +1816,11 @@
       <c r="M22"/>
       <c r="N22"/>
       <c r="O22"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
     </row>
     <row r="23" spans="1:20">
       <c r="K23"/>
@@ -1768,11 +1828,11 @@
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
     </row>
     <row r="24" spans="1:20">
       <c r="K24"/>
@@ -1780,11 +1840,11 @@
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
     </row>
     <row r="25" spans="1:20">
       <c r="K25"/>
@@ -1792,11 +1852,11 @@
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
     </row>
     <row r="26" spans="1:20">
       <c r="K26"/>
@@ -1804,11 +1864,11 @@
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
     </row>
     <row r="27" spans="1:20">
       <c r="K27"/>
@@ -1816,11 +1876,11 @@
       <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
     </row>
     <row r="28" spans="1:20">
       <c r="K28"/>
@@ -1828,11 +1888,11 @@
       <c r="M28"/>
       <c r="N28"/>
       <c r="O28"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20">
       <c r="K29"/>
@@ -1840,11 +1900,11 @@
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
     </row>
     <row r="30" spans="1:20">
       <c r="K30"/>
@@ -1852,11 +1912,11 @@
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
     </row>
     <row r="31" spans="1:20">
       <c r="K31"/>
@@ -1864,11 +1924,11 @@
       <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
     </row>
     <row r="32" spans="1:20">
       <c r="K32"/>
@@ -1876,11 +1936,11 @@
       <c r="M32"/>
       <c r="N32"/>
       <c r="O32"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
     </row>
     <row r="33" spans="11:20">
       <c r="K33"/>
@@ -1888,11 +1948,11 @@
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
     </row>
     <row r="34" spans="11:20">
       <c r="K34"/>
@@ -1900,11 +1960,11 @@
       <c r="M34"/>
       <c r="N34"/>
       <c r="O34"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
     </row>
     <row r="35" spans="11:20">
       <c r="K35"/>
@@ -1912,11 +1972,11 @@
       <c r="M35"/>
       <c r="N35"/>
       <c r="O35"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
     </row>
     <row r="36" spans="11:20">
       <c r="K36"/>
@@ -1924,11 +1984,11 @@
       <c r="M36"/>
       <c r="N36"/>
       <c r="O36"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
     </row>
     <row r="37" spans="11:20">
       <c r="K37"/>
@@ -1936,11 +1996,11 @@
       <c r="M37"/>
       <c r="N37"/>
       <c r="O37"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
     </row>
     <row r="38" spans="11:20">
       <c r="K38"/>
@@ -1948,11 +2008,11 @@
       <c r="M38"/>
       <c r="N38"/>
       <c r="O38"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
     </row>
     <row r="39" spans="11:20">
       <c r="K39"/>
@@ -1960,11 +2020,11 @@
       <c r="M39"/>
       <c r="N39"/>
       <c r="O39"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
     </row>
     <row r="40" spans="11:20">
       <c r="K40"/>
@@ -1972,11 +2032,11 @@
       <c r="M40"/>
       <c r="N40"/>
       <c r="O40"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
     </row>
     <row r="41" spans="11:20">
       <c r="K41"/>
@@ -1984,11 +2044,11 @@
       <c r="M41"/>
       <c r="N41"/>
       <c r="O41"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
     </row>
     <row r="42" spans="11:20">
       <c r="K42"/>
@@ -1996,11 +2056,11 @@
       <c r="M42"/>
       <c r="N42"/>
       <c r="O42"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
     </row>
     <row r="43" spans="11:20">
       <c r="K43"/>
@@ -2008,11 +2068,11 @@
       <c r="M43"/>
       <c r="N43"/>
       <c r="O43"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
     </row>
     <row r="44" spans="11:20">
       <c r="K44"/>
@@ -2020,11 +2080,11 @@
       <c r="M44"/>
       <c r="N44"/>
       <c r="O44"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
     </row>
     <row r="45" spans="11:20">
       <c r="K45"/>
@@ -2032,11 +2092,11 @@
       <c r="M45"/>
       <c r="N45"/>
       <c r="O45"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
     </row>
     <row r="46" spans="11:20">
       <c r="K46"/>
@@ -2044,11 +2104,11 @@
       <c r="M46"/>
       <c r="N46"/>
       <c r="O46"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
     </row>
     <row r="47" spans="11:20">
       <c r="K47"/>
@@ -2056,11 +2116,11 @@
       <c r="M47"/>
       <c r="N47"/>
       <c r="O47"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
     </row>
     <row r="48" spans="11:20">
       <c r="K48"/>
@@ -2111,47 +2171,47 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="32.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="32.83203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="17.6640625" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="14" width="75.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="32.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20" style="2" customWidth="1"/>
+    <col min="5" max="6" width="9.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="32.83203125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="17.6640625" style="2" customWidth="1"/>
+    <col min="11" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="75.6640625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>75</v>
       </c>
       <c r="K1"/>
@@ -2161,16 +2221,16 @@
       <c r="O1"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K2"/>
@@ -2178,23 +2238,23 @@
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K3"/>
@@ -2202,26 +2262,26 @@
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="K4"/>
@@ -2229,29 +2289,29 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K5"/>
@@ -2259,23 +2319,23 @@
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:20" ht="30">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>66</v>
       </c>
       <c r="K6"/>
@@ -2283,23 +2343,23 @@
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
     </row>
     <row r="7" spans="1:20" ht="30">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>67</v>
       </c>
       <c r="K7"/>
@@ -2307,23 +2367,23 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K8"/>
@@ -2331,23 +2391,23 @@
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K9"/>
@@ -2355,23 +2415,23 @@
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>69</v>
       </c>
       <c r="K10"/>
@@ -2379,23 +2439,23 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K11"/>
@@ -2403,23 +2463,23 @@
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20" ht="45">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>58</v>
       </c>
       <c r="K12"/>
@@ -2427,17 +2487,17 @@
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="K13"/>
@@ -2445,17 +2505,17 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
     </row>
     <row r="14" spans="1:20" ht="30">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>74</v>
       </c>
       <c r="K14"/>
@@ -2463,23 +2523,23 @@
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K15"/>
@@ -2487,11 +2547,11 @@
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:20">
       <c r="K16"/>
@@ -2499,11 +2559,11 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
     </row>
     <row r="17" spans="11:20">
       <c r="K17"/>
@@ -2511,11 +2571,11 @@
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
     </row>
     <row r="18" spans="11:20">
       <c r="K18"/>
@@ -2523,11 +2583,11 @@
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
     </row>
     <row r="19" spans="11:20">
       <c r="K19"/>
@@ -2535,11 +2595,11 @@
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
     </row>
     <row r="20" spans="11:20">
       <c r="K20"/>
@@ -2547,11 +2607,11 @@
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
     </row>
     <row r="21" spans="11:20">
       <c r="K21"/>
@@ -2559,11 +2619,11 @@
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
     </row>
     <row r="22" spans="11:20">
       <c r="K22"/>
@@ -2571,11 +2631,11 @@
       <c r="M22"/>
       <c r="N22"/>
       <c r="O22"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
     </row>
     <row r="23" spans="11:20">
       <c r="K23"/>
@@ -2583,11 +2643,11 @@
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
     </row>
     <row r="24" spans="11:20">
       <c r="K24"/>
@@ -2595,11 +2655,11 @@
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
     </row>
     <row r="25" spans="11:20">
       <c r="K25"/>
@@ -2607,11 +2667,11 @@
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
     </row>
     <row r="26" spans="11:20">
       <c r="K26"/>
@@ -2619,11 +2679,11 @@
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
     </row>
     <row r="27" spans="11:20">
       <c r="K27"/>
@@ -2631,11 +2691,11 @@
       <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
     </row>
     <row r="28" spans="11:20">
       <c r="K28"/>
@@ -2643,11 +2703,11 @@
       <c r="M28"/>
       <c r="N28"/>
       <c r="O28"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
     </row>
     <row r="29" spans="11:20">
       <c r="K29"/>
@@ -2655,11 +2715,11 @@
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
     </row>
     <row r="30" spans="11:20">
       <c r="K30"/>
@@ -2667,11 +2727,11 @@
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
     </row>
     <row r="31" spans="11:20">
       <c r="K31"/>
@@ -2679,11 +2739,11 @@
       <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
     </row>
     <row r="32" spans="11:20">
       <c r="K32"/>
@@ -2691,11 +2751,11 @@
       <c r="M32"/>
       <c r="N32"/>
       <c r="O32"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
     </row>
     <row r="33" spans="11:20">
       <c r="K33"/>
@@ -2703,11 +2763,11 @@
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
     </row>
     <row r="34" spans="11:20">
       <c r="K34"/>
@@ -2715,11 +2775,11 @@
       <c r="M34"/>
       <c r="N34"/>
       <c r="O34"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
     </row>
     <row r="35" spans="11:20">
       <c r="K35"/>
@@ -2727,11 +2787,11 @@
       <c r="M35"/>
       <c r="N35"/>
       <c r="O35"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
     </row>
     <row r="36" spans="11:20">
       <c r="K36"/>
@@ -2739,11 +2799,11 @@
       <c r="M36"/>
       <c r="N36"/>
       <c r="O36"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
     </row>
     <row r="37" spans="11:20">
       <c r="K37"/>
@@ -2751,11 +2811,11 @@
       <c r="M37"/>
       <c r="N37"/>
       <c r="O37"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
     </row>
     <row r="38" spans="11:20">
       <c r="K38"/>
@@ -2763,11 +2823,11 @@
       <c r="M38"/>
       <c r="N38"/>
       <c r="O38"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
     </row>
     <row r="39" spans="11:20">
       <c r="K39"/>
@@ -2775,11 +2835,11 @@
       <c r="M39"/>
       <c r="N39"/>
       <c r="O39"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
     </row>
     <row r="40" spans="11:20">
       <c r="K40"/>
@@ -2787,11 +2847,11 @@
       <c r="M40"/>
       <c r="N40"/>
       <c r="O40"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
     </row>
     <row r="41" spans="11:20">
       <c r="K41"/>
@@ -2799,11 +2859,11 @@
       <c r="M41"/>
       <c r="N41"/>
       <c r="O41"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
     </row>
     <row r="42" spans="11:20">
       <c r="K42"/>
@@ -2811,11 +2871,11 @@
       <c r="M42"/>
       <c r="N42"/>
       <c r="O42"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
     </row>
     <row r="43" spans="11:20">
       <c r="K43"/>
@@ -2823,11 +2883,11 @@
       <c r="M43"/>
       <c r="N43"/>
       <c r="O43"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
     </row>
     <row r="44" spans="11:20">
       <c r="K44"/>
@@ -2835,11 +2895,11 @@
       <c r="M44"/>
       <c r="N44"/>
       <c r="O44"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
     </row>
     <row r="45" spans="11:20">
       <c r="K45"/>
@@ -2847,11 +2907,11 @@
       <c r="M45"/>
       <c r="N45"/>
       <c r="O45"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
     </row>
     <row r="46" spans="11:20">
       <c r="K46"/>
@@ -2859,11 +2919,11 @@
       <c r="M46"/>
       <c r="N46"/>
       <c r="O46"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
     </row>
     <row r="47" spans="11:20">
       <c r="K47"/>
@@ -2871,11 +2931,11 @@
       <c r="M47"/>
       <c r="N47"/>
       <c r="O47"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
     </row>
     <row r="48" spans="11:20">
       <c r="K48"/>

</xml_diff>